<commit_message>
Small fix on wrong issue numbers
</commit_message>
<xml_diff>
--- a/docs/sprints.xlsx
+++ b/docs/sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Documents\TU\repositories\SEM\docs\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Documents\TU\repositories\SEM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF02861-1035-40C5-BC02-249F581D0BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0DA8-E587-4998-8EEB-4E75EF8E794A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" activeTab="3" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" activeTab="5" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="93">
   <si>
     <t>User Story #</t>
   </si>
@@ -513,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -598,36 +598,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -693,7 +679,24 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -714,6 +717,9 @@
           <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -754,10 +760,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}" name="Table1" displayName="Table1" ref="A1:H32" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}" name="Table1" displayName="Table1" ref="A1:H32" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:H32" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story " dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{E40A33E7-2DA6-4331-8AE0-2CAF1EE47083}" name="Issue #"/>
     <tableColumn id="2" xr3:uid="{70831594-7EAC-447C-AFB7-FEF4536D539F}" name="Task#"/>
     <tableColumn id="3" xr3:uid="{0DA9E85B-5521-4636-9DE5-1724D932B621}" name="Task assigned to"/>
@@ -771,7 +777,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AA53034-562E-444A-A174-EDCAB48FAF98}" name="Table14" displayName="Table14" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8AA53034-562E-444A-A174-EDCAB48FAF98}" name="Table14" displayName="Table14" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:H1048576" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -788,7 +794,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2BB48A9-B7C9-4465-A694-A1A60DB862A5}" name="Table13" displayName="Table13" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2BB48A9-B7C9-4465-A694-A1A60DB862A5}" name="Table13" displayName="Table13" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:G1048574" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -804,10 +810,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53015D-1831-4CC7-AB65-5D7B71763781}" name="Table16" displayName="Table16" ref="A1:H35" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53015D-1831-4CC7-AB65-5D7B71763781}" name="Table16" displayName="Table16" ref="A1:H35" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:H35" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{60E2564F-7A0E-41C5-B5EF-E3B5C8DF36D3}" name="User Story " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{60E2564F-7A0E-41C5-B5EF-E3B5C8DF36D3}" name="User Story " dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{BE915640-2681-4807-B9F9-EDDB87C59847}" name="Issue #"/>
     <tableColumn id="2" xr3:uid="{D190346C-2729-493C-BBAD-E061FA84D96B}" name="Task#"/>
     <tableColumn id="3" xr3:uid="{ED69C779-D47B-45D0-9B70-47CCE998BEA4}" name="Task assigned to"/>
@@ -821,7 +827,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E492D9C-8291-4D1A-B15F-F7CBDF216488}" name="Table15" displayName="Table15" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E492D9C-8291-4D1A-B15F-F7CBDF216488}" name="Table15" displayName="Table15" ref="A1:G1048574" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:G1048574" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4E6552BF-C350-49D0-BCAD-76EB67F2A002}" name="User Story #"/>
@@ -837,12 +843,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE1F1E48-758A-4606-B3B6-7A9876FFA9A6}" name="Table17" displayName="Table17" ref="A1:H35" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:H35" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE1F1E48-758A-4606-B3B6-7A9876FFA9A6}" name="Table17" displayName="Table17" ref="A1:H37" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H37" xr:uid="{CD2D3C98-B5D1-4498-AAE1-063F5D057A1C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7A20E7DE-AD4A-4D31-B30A-87F953C850B5}" name="User Story " dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{7A20E7DE-AD4A-4D31-B30A-87F953C850B5}" name="User Story " dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{CE04B1C4-291F-469E-8EDA-4B2E50F1E047}" name="Issue #"/>
-    <tableColumn id="2" xr3:uid="{BFE63EB1-FE70-4D90-96B2-63F2704505A1}" name="Task#" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{BFE63EB1-FE70-4D90-96B2-63F2704505A1}" name="Task#" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{8EA413FE-D781-49A6-82E4-A822FAC4AFF5}" name="Task assigned to"/>
     <tableColumn id="4" xr3:uid="{62470DFE-0C6D-4AE3-8552-7F81C0E56895}" name="Estimated Effort"/>
     <tableColumn id="5" xr3:uid="{667E60DB-E809-4D96-9D39-512072F7B841}" name="Actual Effort"/>
@@ -1153,7 +1159,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1267,10 +1273,10 @@
       <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="14">
         <v>3</v>
       </c>
       <c r="C6" s="22"/>
@@ -2159,7 +2165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43D420-8132-4A0A-B840-CA93FDE81F26}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -2993,10 +2999,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC608E94-FFE2-486E-A28F-5ACAAA8D4039}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3118,76 +3124,76 @@
       <c r="G5" s="38"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="16">
-        <v>1</v>
-      </c>
-      <c r="C6" s="41" t="s">
+    <row r="6" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="51" t="s">
         <v>72</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16">
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+    </row>
+    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="21">
+        <v>9</v>
+      </c>
+      <c r="C7" s="53">
+        <v>3.4</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C8" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="21">
-        <v>10</v>
-      </c>
-      <c r="C8" s="44">
-        <v>1.2</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="16">
-        <v>2</v>
-      </c>
-      <c r="C9" s="41">
-        <v>4</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>84</v>
@@ -3196,88 +3202,90 @@
       <c r="G9" s="17"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16">
+    <row r="10" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="21">
+        <v>10</v>
+      </c>
+      <c r="C10" s="44">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="16">
+        <v>2</v>
+      </c>
+      <c r="C11" s="41">
+        <v>4</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="41">
         <v>3</v>
       </c>
-      <c r="C10" s="41">
-        <v>3</v>
-      </c>
-      <c r="D10" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E12" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B13" s="21">
         <v>4</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C13" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="14">
-        <v>8</v>
-      </c>
-      <c r="C12" s="45">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19">
-        <v>8</v>
-      </c>
-      <c r="C13" s="46">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="4"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="14">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="45">
         <v>1</v>
@@ -3292,90 +3300,100 @@
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19">
+        <v>8</v>
+      </c>
+      <c r="C15" s="46">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14">
         <v>7</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C16" s="45">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16">
+        <v>7</v>
+      </c>
+      <c r="C17" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E17" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19">
         <v>7</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C18" s="46">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B19" s="19">
         <v>15</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+      <c r="C19" s="46"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B20" s="21">
         <v>16</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="21">
-        <v>19</v>
-      </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="21">
-        <v>20</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="22"/>
@@ -3384,12 +3402,12 @@
       <c r="G20" s="22"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="27" t="s">
-        <v>26</v>
+    <row r="21" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="21">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="22"/>
@@ -3398,12 +3416,12 @@
       <c r="G21" s="22"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
-        <v>27</v>
+    <row r="22" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="B22" s="21">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C22" s="44"/>
       <c r="D22" s="22"/>
@@ -3414,10 +3432,10 @@
     </row>
     <row r="23" spans="1:8" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="21">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="22"/>
@@ -3427,11 +3445,11 @@
       <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="29" t="s">
-        <v>76</v>
+      <c r="A24" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="B24" s="21">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C24" s="44"/>
       <c r="D24" s="22"/>
@@ -3440,12 +3458,12 @@
       <c r="G24" s="22"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="21">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="22"/>
@@ -3454,12 +3472,12 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="27" t="s">
-        <v>30</v>
+    <row r="26" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="B26" s="21">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C26" s="44"/>
       <c r="D26" s="22"/>
@@ -3468,12 +3486,12 @@
       <c r="G26" s="22"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="21">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="22"/>
@@ -3483,11 +3501,11 @@
       <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="30" t="s">
-        <v>32</v>
+      <c r="A28" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="B28" s="21">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="22"/>
@@ -3497,11 +3515,11 @@
       <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="30" t="s">
-        <v>33</v>
+      <c r="A29" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="B29" s="21">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C29" s="44"/>
       <c r="D29" s="22"/>
@@ -3512,10 +3530,10 @@
     </row>
     <row r="30" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="21">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="44"/>
       <c r="D30" s="22"/>
@@ -3524,12 +3542,12 @@
       <c r="G30" s="22"/>
       <c r="H30" s="23"/>
     </row>
-    <row r="31" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="21">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="22"/>
@@ -3540,10 +3558,10 @@
     </row>
     <row r="32" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="21">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="22"/>
@@ -3552,12 +3570,12 @@
       <c r="G32" s="22"/>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="21">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="22"/>
@@ -3566,12 +3584,12 @@
       <c r="G33" s="22"/>
       <c r="H33" s="23"/>
     </row>
-    <row r="34" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="21">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="22"/>
@@ -3582,10 +3600,10 @@
     </row>
     <row r="35" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="21">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="22"/>
@@ -3594,13 +3612,41 @@
       <c r="G35" s="22"/>
       <c r="H35" s="23"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="26"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="26"/>
+    <row r="36" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="21">
+        <v>28</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="21">
+        <v>29</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="23"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add the activities of Ravi to the sprint
</commit_message>
<xml_diff>
--- a/docs/sprints.xlsx
+++ b/docs/sprints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauli\Documents\TU\repositories\SEM\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E0DA8-E587-4998-8EEB-4E75EF8E794A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52937299-45E0-4BA4-A777-7B753FAC52A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" activeTab="5" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="671" activeTab="3" xr2:uid="{58667ADA-671B-4355-9B89-7418DDCFDFF4}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="95">
   <si>
     <t>User Story #</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>TA Hiring System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create class diagramm for the design patterns, do assignment 1 part2(apart from coding) and finish assignment 1 part 1  </t>
+  </si>
+  <si>
+    <t>iarina, gijs, vincent,ravi,andrei</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -860,7 +866,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1933,7 +1939,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,7 +2044,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="D4" s="8">
         <v>5</v>
@@ -2165,15 +2171,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D43D420-8132-4A0A-B840-CA93FDE81F26}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="81.21875" customWidth="1"/>
     <col min="4" max="4" width="35.5546875" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
@@ -2272,14 +2278,20 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="E5" s="8">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="K5" t="s">
         <v>8</v>
@@ -2735,13 +2747,13 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" customWidth="1"/>
     <col min="3" max="3" width="27.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
@@ -3001,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC608E94-FFE2-486E-A28F-5ACAAA8D4039}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>